<commit_message>
Anforderungen angepasst + cBFill
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Anforderungen</t>
   </si>
@@ -100,12 +100,15 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Zitate können angezeigt werden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -206,7 +209,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -221,8 +224,42 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="4"/>
+      <tableStyleElement type="headerRow" dxfId="3"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -277,7 +314,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -312,7 +349,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -489,7 +526,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -497,19 +534,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,210 +557,219 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>18</v>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>21</v>
+    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
+    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+    </row>
+    <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A27" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A15:A21 A2:A13">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A16:A22 A2:A14">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>B2="x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>B13="x"</formula>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>B14="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -732,31 +778,31 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<sisl xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="http://www.boldonjames.com/2008/01/sie/internal/label" sislVersion="0" policy="5e216652-7cb1-42d3-a22f-fb5c7f348db5" origin="userSelected">
+  <element uid="id_classification_nonbusiness" value=""/>
+</sisl>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <WrappedLabelHistory xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="http://www.boldonjames.com/2016/02/Classifier/internal/wrappedLabelHistory">
   <Value>PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXMtYXNjaWkiPz48bGFiZWxIaXN0b3J5IHhtbG5zOnhzaT0iaHR0cDovL3d3dy53My5vcmcvMjAwMS9YTUxTY2hlbWEtaW5zdGFuY2UiIHhtbG5zOnhzZD0iaHR0cDovL3d3dy53My5vcmcvMjAwMS9YTUxTY2hlbWEiIHhtbG5zPSJodHRwOi8vd3d3LmJvbGRvbmphbWVzLmNvbS8yMDE2LzAyL0NsYXNzaWZpZXIvaW50ZXJuYWwvbGFiZWxIaXN0b3J5Ij48aXRlbT48c2lzbCBzaXNsVmVyc2lvbj0iMCIgcG9saWN5PSI1ZTIxNjY1Mi03Y2IxLTQyZDMtYTIyZi1mYjVjN2YzNDhkYjUiIG9yaWdpbj0idXNlclNlbGVjdGVkIj48ZWxlbWVudCB1aWQ9ImlkX2NsYXNzaWZpY2F0aW9uX25vbmJ1c2luZXNzIiB2YWx1ZT0iIiB4bWxucz0iaHR0cDovL3d3dy5ib2xkb25qYW1lcy5jb20vMjAwOC8wMS9zaWUvaW50ZXJuYWwvbGFiZWwiIC8+PC9zaXNsPjxVc2VyTmFtZT5PQUFEXHFkODg5PC9Vc2VyTmFtZT48RGF0ZVRpbWU+OS8xMy8yMDE4IDY6NDY6MjIgQU08L0RhdGVUaW1lPjxMYWJlbFN0cmluZz5QdWJsaWM8L0xhYmVsU3RyaW5nPjwvaXRlbT48L2xhYmVsSGlzdG9yeT4=</Value>
 </WrappedLabelHistory>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<sisl xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="http://www.boldonjames.com/2008/01/sie/internal/label" sislVersion="0" policy="5e216652-7cb1-42d3-a22f-fb5c7f348db5" origin="userSelected">
-  <element uid="id_classification_nonbusiness" value=""/>
-</sisl>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{300B9EDB-F9C6-40B4-AE9F-BA40CFAD302F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA25C00C-19BF-4631-BD00-2DF94E815248}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2016/02/Classifier/internal/wrappedLabelHistory"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{300B9EDB-F9C6-40B4-AE9F-BA40CFAD302F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ABC Analyse & Haken
ABC Analyse von Herrn Grüning eingetragen.
Login abgehakt
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Anforderungen</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -497,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,7 +521,7 @@
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -528,8 +540,11 @@
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -537,8 +552,11 @@
       <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -546,8 +564,11 @@
       <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -555,8 +576,11 @@
       <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -564,17 +588,25 @@
       <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -582,8 +614,11 @@
       <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -592,7 +627,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -601,7 +636,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -610,7 +645,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -619,7 +654,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -628,7 +663,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -636,8 +671,11 @@
       <c r="C14" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -645,8 +683,11 @@
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -654,8 +695,11 @@
       <c r="C16" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -663,8 +707,11 @@
       <c r="C17" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -673,7 +720,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
@@ -682,7 +729,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -691,7 +738,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -700,19 +747,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
     </row>
   </sheetData>
@@ -753,7 +800,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{300B9EDB-F9C6-40B4-AE9F-BA40CFAD302F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67A0BF7B-9B87-493C-8313-FC7959BE95CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>